<commit_message>
Upgrade version 4 20250211
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Futures of Flowiee.xlsx
+++ b/src/main/resources/static/Futures of Flowiee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\FW_PMS\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B99FB-0435-4A00-A0E4-D59633CA017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5399C826-AE47-48DF-BE21-DF9D3F5DD6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="3" xr2:uid="{7E065712-1017-4994-91F5-97AFA9456CE1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="1142">
   <si>
     <t>Quản lý người dùng</t>
   </si>
@@ -12036,8 +12036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3403C1F-7924-47A2-BC02-BD259991C3B3}">
   <dimension ref="B2:D418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="B413" sqref="B413"/>
+    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="B263" sqref="B263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -13486,160 +13486,166 @@
         <v>967</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B257" s="10" t="s">
         <v>968</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B258" s="12"/>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B259" s="12" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B260" s="12" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B261" s="12" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B262" s="12" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B263" s="12" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B264" s="12" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B265" s="12" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B266" s="12" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B267" s="12" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B268" s="12" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B269" s="12" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B270" s="12" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C270" s="11" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="271" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B271" s="12" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B272" s="12" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B273" s="12" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B274" s="12" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C274" s="11" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="275" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B275" s="12" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B276" s="12" t="s">
         <v>986</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B277" s="12" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B278" s="12" t="s">
         <v>988</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B279" s="12" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B280" s="12" t="s">
         <v>990</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B281" s="12" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B282" s="12" t="s">
         <v>992</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B283" s="12" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B284" s="12" t="s">
         <v>994</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B285" s="12" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B286" s="12" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B287" s="12" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B288" s="12" t="s">
         <v>998</v>
       </c>

</xml_diff>